<commit_message>
tests, documentation and errror handling written for ISRate
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR.xlsx
@@ -5,24 +5,25 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annabel.Westermann\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26157586-1C9A-4014-9B3A-152232D3B23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350B830-A37B-42B4-BC7E-33646F468262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="719" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="719" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
     <sheet name="testdata_multiarea_isr" sheetId="15" r:id="rId2"/>
-    <sheet name="testdata_multiarea" sheetId="5" r:id="rId3"/>
-    <sheet name="testdata_1976" sheetId="12" r:id="rId4"/>
-    <sheet name="refdata" sheetId="14" r:id="rId5"/>
-    <sheet name="testresults_ISR" sheetId="13" r:id="rId6"/>
-    <sheet name="testresults_DSR" sheetId="4" r:id="rId7"/>
-    <sheet name="testdata_err1" sheetId="7" r:id="rId8"/>
-    <sheet name="testdata_err2" sheetId="8" r:id="rId9"/>
-    <sheet name="testdata_err3" sheetId="9" r:id="rId10"/>
+    <sheet name="testdata_multiarea_lookup" sheetId="17" r:id="rId3"/>
+    <sheet name="testdata_multiarea" sheetId="5" r:id="rId4"/>
+    <sheet name="testdata_1976" sheetId="12" r:id="rId5"/>
+    <sheet name="refdata" sheetId="14" r:id="rId6"/>
+    <sheet name="testresults_ISR" sheetId="13" r:id="rId7"/>
+    <sheet name="testresults_DSR" sheetId="4" r:id="rId8"/>
+    <sheet name="testdata_err1" sheetId="7" r:id="rId9"/>
+    <sheet name="testdata_err2" sheetId="8" r:id="rId10"/>
+    <sheet name="testdata_err3" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="58">
   <si>
     <t>0-4</t>
   </si>
@@ -2678,6 +2679,467 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
+        <v>127</v>
+      </c>
+      <c r="C2" s="5">
+        <v>636</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="10">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="4">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="4">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="4">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="4">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4">
+        <v>91</v>
+      </c>
+      <c r="C20" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="7">
+        <v>12</v>
+      </c>
+      <c r="C21" s="8">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="4">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="4">
+        <v>8</v>
+      </c>
+      <c r="C27" s="5">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="C31" s="5">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="4">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="4">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="4">
+        <v>8</v>
+      </c>
+      <c r="C34" s="5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="4">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="4">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="4">
+        <v>5</v>
+      </c>
+      <c r="C37" s="5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="4">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="4">
+        <v>4</v>
+      </c>
+      <c r="C39" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:D22"/>
@@ -2993,8 +3455,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4160,6 +4622,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3582517-898A-4E83-8FF5-D6610E682911}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>91</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D58"/>
@@ -4988,7 +5508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D22"/>
@@ -5292,7 +5812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D20"/>
@@ -5529,12 +6049,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -6114,7 +6634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J9"/>
@@ -6398,7 +6918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D22"/>
@@ -6708,465 +7228,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:F41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="4">
-        <v>127</v>
-      </c>
-      <c r="C2" s="5">
-        <v>636</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="10">
-        <v>25</v>
-      </c>
-      <c r="C3" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="10">
-        <v>18</v>
-      </c>
-      <c r="C4" s="11">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="4">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="4">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="4">
-        <v>48</v>
-      </c>
-      <c r="C8" s="5">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="4">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="4">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="4">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="4">
-        <v>32</v>
-      </c>
-      <c r="C12" s="5">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="4">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="4">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="4">
-        <v>65</v>
-      </c>
-      <c r="C15" s="5">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="4">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4">
-        <v>68</v>
-      </c>
-      <c r="C17" s="5">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="4">
-        <v>74</v>
-      </c>
-      <c r="C18" s="5">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="4">
-        <v>82</v>
-      </c>
-      <c r="C19" s="5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4">
-        <v>91</v>
-      </c>
-      <c r="C20" s="5">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="7">
-        <v>12</v>
-      </c>
-      <c r="C21" s="8">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="4">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="4">
-        <v>3</v>
-      </c>
-      <c r="C23" s="5">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="4">
-        <v>2</v>
-      </c>
-      <c r="C24" s="5">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="4">
-        <v>3</v>
-      </c>
-      <c r="C25" s="5">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="4">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="4">
-        <v>8</v>
-      </c>
-      <c r="C27" s="5">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="4">
-        <v>2</v>
-      </c>
-      <c r="C28" s="5">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="4">
-        <v>2</v>
-      </c>
-      <c r="C29" s="5">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="4">
-        <v>3</v>
-      </c>
-      <c r="C30" s="5">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="4">
-        <v>4</v>
-      </c>
-      <c r="C31" s="5">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="4">
-        <v>5</v>
-      </c>
-      <c r="C32" s="5">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="4">
-        <v>6</v>
-      </c>
-      <c r="C33" s="5">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="4">
-        <v>8</v>
-      </c>
-      <c r="C34" s="5">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="4">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="4">
-        <v>6</v>
-      </c>
-      <c r="C36" s="5">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="4">
-        <v>5</v>
-      </c>
-      <c r="C37" s="5">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="4">
-        <v>5</v>
-      </c>
-      <c r="C38" s="5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="4">
-        <v>4</v>
-      </c>
-      <c r="C39" s="5">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Ads test for DSR with non-independent events. Suppresses warnings in test_phe_dsr. Updates expect_equivalent to expect_equal in life expectancy tests.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annabel.Westermann\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350B830-A37B-42B4-BC7E-33646F468262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEFDCE4-E6FC-40DB-8FFF-3F562F7B508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="719" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="719" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
     <sheet name="testdata_multiarea_isr" sheetId="15" r:id="rId2"/>
     <sheet name="testdata_multiarea_lookup" sheetId="17" r:id="rId3"/>
     <sheet name="testdata_multiarea" sheetId="5" r:id="rId4"/>
-    <sheet name="testdata_1976" sheetId="12" r:id="rId5"/>
-    <sheet name="refdata" sheetId="14" r:id="rId6"/>
-    <sheet name="testresults_ISR" sheetId="13" r:id="rId7"/>
-    <sheet name="testresults_DSR" sheetId="4" r:id="rId8"/>
-    <sheet name="testdata_err1" sheetId="7" r:id="rId9"/>
-    <sheet name="testdata_err2" sheetId="8" r:id="rId10"/>
-    <sheet name="testdata_err3" sheetId="9" r:id="rId11"/>
+    <sheet name="testdata_nonindepe" sheetId="18" r:id="rId5"/>
+    <sheet name="testdata_1976" sheetId="12" r:id="rId6"/>
+    <sheet name="refdata" sheetId="14" r:id="rId7"/>
+    <sheet name="testresults_ISR" sheetId="13" r:id="rId8"/>
+    <sheet name="testresults_DSR" sheetId="4" r:id="rId9"/>
+    <sheet name="testdata_err1" sheetId="7" r:id="rId10"/>
+    <sheet name="testdata_err2" sheetId="8" r:id="rId11"/>
+    <sheet name="testdata_err3" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="68">
   <si>
     <t>0-4</t>
   </si>
@@ -219,6 +220,36 @@
   <si>
     <t>indirectly standardised ratio x 1</t>
   </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>testdata_nonind_small</t>
+  </si>
+  <si>
+    <t>testdata_nonind_dummy</t>
+  </si>
+  <si>
+    <t>testdata_nonind_big</t>
+  </si>
+  <si>
+    <t>00-04</t>
+  </si>
+  <si>
+    <t>05-09</t>
+  </si>
+  <si>
+    <t>Dobson, with confidence adjusted for non-independent events</t>
+  </si>
 </sst>
 </file>
 
@@ -316,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -423,6 +454,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2679,6 +2716,318 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>127</v>
+      </c>
+      <c r="C2" s="5">
+        <v>636</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11">
+        <v>558</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11">
+        <v>609</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>543</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>384</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21">
+        <v>-26</v>
+      </c>
+      <c r="C7" s="5">
+        <v>594</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5">
+        <v>669</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5">
+        <v>843</v>
+      </c>
+      <c r="D9" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5">
+        <v>660</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>576</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5">
+        <v>606</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>522</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5">
+        <v>426</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5">
+        <v>273</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5">
+        <v>300</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5">
+        <v>288</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5">
+        <v>153</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5">
+        <v>123</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>91</v>
+      </c>
+      <c r="C20" s="5">
+        <v>207</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F41"/>
@@ -3139,7 +3488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:D22"/>
@@ -3455,8 +3804,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5509,6 +5858,1605 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BA0C53-A024-4465-9ADC-66E4AB5F6507}">
+  <dimension ref="A1:H58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <v>127</v>
+      </c>
+      <c r="D2">
+        <v>636</v>
+      </c>
+      <c r="E2">
+        <f>$C2-($F2*2)-($G2*3)-($H2*4)</f>
+        <v>75</v>
+      </c>
+      <c r="F2">
+        <f>ROUND(0.25*$C2/2,0)</f>
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(0.1*$C2/3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>ROUND(0.05*$C2/4,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>558</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E20" si="0">$C3-($F3*2)-($G3*3)-($H3*4)</f>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F20" si="1">ROUND(0.25*$C3/2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G20" si="2">ROUND(0.1*$C3/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H20" si="3">ROUND(0.05*$C3/4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>609</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>543</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>384</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>594</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>669</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>843</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>660</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>576</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>606</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>522</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>426</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <v>273</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>300</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>288</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>153</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>82</v>
+      </c>
+      <c r="D19">
+        <v>123</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>91</v>
+      </c>
+      <c r="D20">
+        <v>207</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21">
+        <v>127</v>
+      </c>
+      <c r="D21">
+        <v>636</v>
+      </c>
+      <c r="E21">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>558</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>18</v>
+      </c>
+      <c r="D23">
+        <v>609</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>543</v>
+      </c>
+      <c r="E24">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>384</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>594</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>669</v>
+      </c>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>843</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>660</v>
+      </c>
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>576</v>
+      </c>
+      <c r="E30">
+        <v>23</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>32</v>
+      </c>
+      <c r="D31">
+        <v>606</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <v>522</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>45</v>
+      </c>
+      <c r="D33">
+        <v>426</v>
+      </c>
+      <c r="E33">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>7</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>65</v>
+      </c>
+      <c r="D34">
+        <v>273</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>300</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>68</v>
+      </c>
+      <c r="D36">
+        <v>288</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>74</v>
+      </c>
+      <c r="D37">
+        <v>153</v>
+      </c>
+      <c r="E37">
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>82</v>
+      </c>
+      <c r="D38">
+        <v>123</v>
+      </c>
+      <c r="E38">
+        <v>29</v>
+      </c>
+      <c r="F38">
+        <v>19</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39">
+        <v>91</v>
+      </c>
+      <c r="D39">
+        <v>207</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
+        <v>21</v>
+      </c>
+      <c r="G39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40">
+        <v>636</v>
+      </c>
+      <c r="E40">
+        <f>$C40-($F40*2)-($G40*3)-($H40*4)</f>
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="F40:F58" si="4">ROUND(0.1*$C40/2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:G58" si="5">ROUND(0.25*$C40/3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:H58" si="6">ROUND(0.05*$C40/4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>558</v>
+      </c>
+      <c r="E41">
+        <f>$C41-($F41*2)-($G41*3)-($H41*4)</f>
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>609</v>
+      </c>
+      <c r="E42">
+        <f>$C42-($F42*2)-($G42*3)-($H42*4)</f>
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="38">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>543</v>
+      </c>
+      <c r="E43" s="38">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>384</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ref="E44:E58" si="7">$C44-($F44*2)-($G44*3)-($H44*4)</f>
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>594</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>669</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>843</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>660</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>576</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>606</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>522</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>426</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>273</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>300</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>288</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56">
+        <v>153</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>123</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>207</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B4 B23 B42" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D22"/>
@@ -5812,7 +7760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D20"/>
@@ -6049,7 +7997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K17"/>
@@ -6634,18 +8582,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
@@ -6912,317 +8860,101 @@
         <v>33</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>127</v>
-      </c>
-      <c r="C2" s="5">
-        <v>636</v>
-      </c>
-      <c r="D2" s="6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10">
-        <v>25</v>
-      </c>
-      <c r="C3" s="11">
-        <v>558</v>
-      </c>
-      <c r="D3" s="12">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10">
-        <v>18</v>
-      </c>
-      <c r="C4" s="11">
-        <v>609</v>
-      </c>
-      <c r="D4" s="12">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5">
-        <v>543</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5">
-        <v>384</v>
-      </c>
-      <c r="D6" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="21">
-        <v>-26</v>
-      </c>
-      <c r="C7" s="5">
-        <v>594</v>
-      </c>
-      <c r="D7" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>48</v>
-      </c>
-      <c r="C8" s="5">
-        <v>669</v>
-      </c>
-      <c r="D8" s="6">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5">
-        <v>843</v>
-      </c>
-      <c r="D9" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5">
-        <v>660</v>
-      </c>
-      <c r="D10" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5">
-        <v>576</v>
-      </c>
-      <c r="D11" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4">
-        <v>32</v>
-      </c>
-      <c r="C12" s="5">
-        <v>606</v>
-      </c>
-      <c r="D12" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5">
-        <v>522</v>
-      </c>
-      <c r="D13" s="6">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5">
-        <v>426</v>
-      </c>
-      <c r="D14" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4">
-        <v>65</v>
-      </c>
-      <c r="C15" s="5">
-        <v>273</v>
-      </c>
-      <c r="D15" s="6">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5">
-        <v>300</v>
-      </c>
-      <c r="D16" s="6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4">
-        <v>68</v>
-      </c>
-      <c r="C17" s="5">
-        <v>288</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>74</v>
-      </c>
-      <c r="C18" s="5">
-        <v>153</v>
-      </c>
-      <c r="D18" s="6">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4">
-        <v>82</v>
-      </c>
-      <c r="C19" s="5">
-        <v>123</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
-        <v>91</v>
-      </c>
-      <c r="C20" s="5">
-        <v>207</v>
-      </c>
-      <c r="D20" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>895</v>
+      </c>
+      <c r="C10">
+        <v>8970</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10430.24799147</v>
+      </c>
+      <c r="E10" s="18">
+        <v>9532.9497786200009</v>
+      </c>
+      <c r="F10" s="18">
+        <v>11373.074832980001</v>
+      </c>
+      <c r="G10" s="18">
+        <v>9036.2563135700002</v>
+      </c>
+      <c r="H10" s="18">
+        <v>11929.24980749</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <v>895</v>
+      </c>
+      <c r="C11">
+        <v>8970</v>
+      </c>
+      <c r="D11" s="18">
+        <v>10430.24799147</v>
+      </c>
+      <c r="E11" s="18">
+        <v>9512.2988375200002</v>
+      </c>
+      <c r="F11" s="18">
+        <v>11394.77359633</v>
+      </c>
+      <c r="G11" s="18">
+        <v>9004.1741812100008</v>
+      </c>
+      <c r="H11" s="18">
+        <v>11963.748704039999</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>89</v>
+      </c>
+      <c r="C12">
+        <v>8970</v>
+      </c>
+      <c r="D12" s="18">
+        <v>1082.9541984099999</v>
+      </c>
+      <c r="E12" s="18">
+        <v>817.68609755</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1393.5588492700001</v>
+      </c>
+      <c r="G12" s="18">
+        <v>684.16751792000002</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1585.4964559299999</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update DSR error handling tests
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia.BoxPower\Documents\R-projects\Packages\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEFDCE4-E6FC-40DB-8FFF-3F562F7B508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E08DDD-C42A-4A74-8CD4-E102C9B22548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="719" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" tabRatio="719" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="testdata_err1" sheetId="7" r:id="rId10"/>
     <sheet name="testdata_err2" sheetId="8" r:id="rId11"/>
     <sheet name="testdata_err3" sheetId="9" r:id="rId12"/>
+    <sheet name="testdata_err4" sheetId="19" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="68">
   <si>
     <t>0-4</t>
   </si>
@@ -261,7 +262,7 @@
     <numFmt numFmtId="166" formatCode="??,??0"/>
     <numFmt numFmtId="167" formatCode="?,???,??0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +320,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -347,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -460,6 +467,14 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3799,6 +3814,316 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009B96CD-357C-4E9F-87E3-30A41B33D8F7}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>127</v>
+      </c>
+      <c r="C2" s="5">
+        <v>636</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="42">
+        <v>558</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11">
+        <v>609</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>543</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>384</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>594</v>
+      </c>
+      <c r="D7" s="43">
+        <v>-6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5">
+        <v>669</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5">
+        <v>843</v>
+      </c>
+      <c r="D9" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5">
+        <v>660</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>576</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5">
+        <v>606</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>522</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5">
+        <v>426</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5">
+        <v>273</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5">
+        <v>300</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5">
+        <v>288</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5">
+        <v>153</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5">
+        <v>123</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>91</v>
+      </c>
+      <c r="C20" s="5">
+        <v>207</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
@@ -8587,7 +8912,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>